<commit_message>
Add note re duplicates
</commit_message>
<xml_diff>
--- a/reference-files/excel-template.xlsx
+++ b/reference-files/excel-template.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="164">
   <si>
     <t>Scotland</t>
   </si>
@@ -622,6 +622,21 @@
   <si>
     <t>PDS started within 12 months and not yet been delivered for a minimum of 11 months.</t>
   </si>
+  <si>
+    <t>For a relatively small number of individuals, multiple records were submitted and to avoid counting these service users more than once, the following rules were applied to select only one record per individual:</t>
+  </si>
+  <si>
+    <t>There also exists a Service Level Agreement between NHS Highland and NHS Greater Glasgow &amp; Clyde health boards, where some PDS is provided to Argyll &amp; Bute residents by West Dunbartonshire IJB. The support provided to these service users has been apportioned to NHS Highland in this report, as part of the LDP Standard is a population based measure, and so by not including these Argyll &amp; Bute residents this figure may be skewed.</t>
+  </si>
+  <si>
+    <t>1.    Keep record with earliest diagnosis date. If these are the same, then;</t>
+  </si>
+  <si>
+    <t>2.    Keep record with termination reason that service user has moved to a different Health Board area. If no record was terminated for this reason, then;</t>
+  </si>
+  <si>
+    <t>3.    Keep record with earliest first contact date.</t>
+  </si>
 </sst>
 </file>
 
@@ -954,7 +969,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1208,6 +1223,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -11817,7 +11835,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFC32"/>
+  <dimension ref="A1:XFC38"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -28402,10 +28420,105 @@
         <v>144</v>
       </c>
     </row>
+    <row r="34" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="124" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="124"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="124"/>
+      <c r="F34" s="124"/>
+      <c r="G34" s="124"/>
+      <c r="H34" s="124"/>
+      <c r="I34" s="124"/>
+      <c r="J34" s="124"/>
+      <c r="K34" s="124"/>
+      <c r="L34" s="124"/>
+      <c r="M34" s="124"/>
+      <c r="N34" s="124"/>
+      <c r="O34" s="124"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B35" s="124" t="s">
+        <v>161</v>
+      </c>
+      <c r="C35" s="124"/>
+      <c r="D35" s="124"/>
+      <c r="E35" s="124"/>
+      <c r="F35" s="124"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="124"/>
+      <c r="I35" s="124"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="124"/>
+      <c r="M35" s="124"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="124"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B36" s="124" t="s">
+        <v>162</v>
+      </c>
+      <c r="C36" s="124"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="124"/>
+      <c r="I36" s="124"/>
+      <c r="J36" s="124"/>
+      <c r="K36" s="124"/>
+      <c r="L36" s="124"/>
+      <c r="M36" s="124"/>
+      <c r="N36" s="124"/>
+      <c r="O36" s="124"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B37" s="124" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="124"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="124"/>
+      <c r="F37" s="124"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="124"/>
+      <c r="I37" s="124"/>
+      <c r="J37" s="124"/>
+      <c r="K37" s="124"/>
+      <c r="L37" s="124"/>
+      <c r="M37" s="124"/>
+      <c r="N37" s="124"/>
+      <c r="O37" s="124"/>
+    </row>
+    <row r="38" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="124" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="124"/>
+      <c r="D38" s="124"/>
+      <c r="E38" s="124"/>
+      <c r="F38" s="124"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="124"/>
+      <c r="I38" s="124"/>
+      <c r="J38" s="124"/>
+      <c r="K38" s="124"/>
+      <c r="L38" s="124"/>
+      <c r="M38" s="124"/>
+      <c r="N38" s="124"/>
+      <c r="O38" s="124"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="B37:O37"/>
+    <mergeCell ref="B38:O38"/>
     <mergeCell ref="C29:I29"/>
     <mergeCell ref="C30:I30"/>
+    <mergeCell ref="B34:O34"/>
+    <mergeCell ref="B35:O35"/>
+    <mergeCell ref="B36:O36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Amendments to excel tables
</commit_message>
<xml_diff>
--- a/reference-files/excel-template.xlsx
+++ b/reference-files/excel-template.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="176">
   <si>
     <t>Scotland</t>
   </si>
@@ -324,9 +324,6 @@
     <t>Methodology</t>
   </si>
   <si>
-    <t>1. These tables are supplementary to the full publication report which can be found at:</t>
-  </si>
-  <si>
     <t>The LDP standard is reported in two parts:</t>
   </si>
   <si>
@@ -376,15 +373,6 @@
   </si>
   <si>
     <t>LDP standard met + Exempt from LD standard + LDP standard not met</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. The Scottish Government published their third national dementia strategy in 2017. This included the commitment to extend and embed dementia post-diagnostic support. In order to effectively monitor the delivery of post-diagnosis support a national local delivery plan (LDP) standard was introduced for all those newly diagnosed with dementia to receive a minimum of one year’s post-diagnostic support. </t>
-  </si>
-  <si>
-    <t>5. Health Board level estimates of the number of people newly diagnosed with dementia (incidence) used in Tab 5 are from the paper 'Estimated and Projected Diagnosis Rates for Dementia in Scotland:  2014-2020', published by the Scottish Government in December 2016. Note that these estimations are subject to the limitations detailed within the paper.</t>
-  </si>
-  <si>
-    <t>4. Due to the change in definitions, improvements in data quality and refinements to the method used to calculate the LDP standard, information presented in this publication is not comparable to previously published information relating to the dementia post-diagnostic support LDP standard.</t>
   </si>
   <si>
     <t xml:space="preserve">LDP standard achieved (%) =   </t>
@@ -662,6 +650,60 @@
   <si>
     <t>Tab 3: Number and percentage of people referred for dementia post-diagnostic support who received a minimum of one year’s support;</t>
   </si>
+  <si>
+    <t>Information presented in this publication is not comparable to information published for time periods prior to 2016/17.</t>
+  </si>
+  <si>
+    <t>As a result of the COVID-19 pandemic, some areas have reported difficulties in updating their data systems which are required to provide the dementia PDS dataset, however it is not anticipated that this has a large impact on the data presented in this report.</t>
+  </si>
+  <si>
+    <t>Aberdeen City Health &amp; Social Care Partnership ceased its contract with Alzheimer Scotland during 2019 and introduced an in house dementia PDS service. This transition resulted in some PDS cases being terminated by Alzheimer Scotland earlier than 12 months and therefore not meeting the LDP standard. As part of the transition, individuals were contacted to ask if they still wanted to receive PDS which was then provided by the in house service, if required. This should be taken into account when interpreting figures for 2018/19.</t>
+  </si>
+  <si>
+    <t>2018/19 figures for NHS Grampian and Aberdeen City are affected by a change in service provision of PDS within Aberdeen City during 2019. See Notes tab for further information.</t>
+  </si>
+  <si>
+    <t>2018/19 figures for NHS Grampian are affected by a change in service provision of PDS within Aberdeen City during 2019. See Notes tab for further information.</t>
+  </si>
+  <si>
+    <t>2018/19 figures are affected by a change in service provision of PDS within Aberdeen City during 2019. See Notes tab for further information.</t>
+  </si>
+  <si>
+    <t>2018/19 figures for Aberdeen City are affected by a change in service provision of PDS during 2019. See Notes tab for further information.</t>
+  </si>
+  <si>
+    <t>1/</t>
+  </si>
+  <si>
+    <t>These tables are supplementary to the full publication report which can be found at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Scottish Government published their third national dementia strategy in 2017. This included the commitment to extend and embed dementia post-diagnostic support. In order to effectively monitor the delivery of post-diagnosis support a national local delivery plan (LDP) standard was introduced for all those newly diagnosed with dementia to receive a minimum of one year’s post-diagnostic support. </t>
+  </si>
+  <si>
+    <t>2/</t>
+  </si>
+  <si>
+    <t>3/</t>
+  </si>
+  <si>
+    <t>Health Board level estimates of the number of people newly diagnosed with dementia (incidence) used in Tab 5 are from the paper 'Estimated and Projected Diagnosis Rates for Dementia in Scotland:  2014-2020', published by the Scottish Government in December 2016. Note that these estimations are subject to the limitations detailed within the paper.</t>
+  </si>
+  <si>
+    <t>4/</t>
+  </si>
+  <si>
+    <t>5/</t>
+  </si>
+  <si>
+    <t>6/</t>
+  </si>
+  <si>
+    <t>7/</t>
+  </si>
+  <si>
+    <t>8/</t>
+  </si>
 </sst>
 </file>
 
@@ -672,7 +714,7 @@
     <numFmt numFmtId="165" formatCode="?0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,6 +941,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1058,7 +1106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -1274,13 +1322,41 @@
     </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="2"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1301,23 +1377,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1368,7 +1430,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1487,7 +1548,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1808,7 +1868,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1948,7 +2007,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2371,7 +2429,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2673,7 +2730,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2764,7 +2820,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2883,7 +2938,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3166,7 +3220,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3285,7 +3338,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3570,7 +3622,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3689,7 +3740,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3954,7 +4004,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4073,7 +4122,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4340,7 +4388,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4459,7 +4506,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4779,7 +4825,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5079,7 +5124,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10317,7 +10361,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="Drop Down 1" hidden="1">
+            <xdr:cNvPr id="2" name="Drop Down 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
@@ -10359,13 +10403,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>161927</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -10559,7 +10603,7 @@
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="Drop Down 1" hidden="1">
+            <xdr:cNvPr id="2" name="Drop Down 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s13313"/>
@@ -10601,13 +10645,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>9527</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11083,13 +11127,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>657226</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11115,13 +11159,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1066801</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11357,13 +11401,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -11389,13 +11433,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -12192,14 +12236,14 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:R49"/>
+  <dimension ref="B2:S47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
     <col min="4" max="17" width="9.85546875" customWidth="1"/>
     <col min="18" max="18" width="9.7109375" customWidth="1"/>
@@ -12280,69 +12324,69 @@
     </row>
     <row r="8" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="104" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="103" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="103" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="103" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="113" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="7" t="s">
+    <row r="13" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="103" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="112" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="112" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="112" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="112" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="112" t="s">
-        <v>154</v>
+      <c r="C15" s="103" t="s">
+        <v>150</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="112" t="s">
-        <v>155</v>
+      <c r="C16" s="103" t="s">
+        <v>151</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -12371,7 +12415,10 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>96</v>
+        <v>165</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12381,181 +12428,270 @@
       <c r="B22" s="1"/>
     </row>
     <row r="23" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="105" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="105"/>
-      <c r="L23" s="105"/>
-      <c r="M23" s="105"/>
-      <c r="N23" s="105"/>
-      <c r="O23" s="105"/>
-      <c r="P23" s="105"/>
-      <c r="Q23" s="105"/>
-      <c r="R23" s="105"/>
+      <c r="B23" s="114" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" s="118" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="118"/>
+      <c r="E23" s="118"/>
+      <c r="F23" s="118"/>
+      <c r="G23" s="118"/>
+      <c r="H23" s="118"/>
+      <c r="I23" s="118"/>
+      <c r="J23" s="118"/>
+      <c r="K23" s="118"/>
+      <c r="L23" s="118"/>
+      <c r="M23" s="118"/>
+      <c r="N23" s="118"/>
+      <c r="O23" s="118"/>
+      <c r="P23" s="118"/>
+      <c r="Q23" s="118"/>
+      <c r="R23" s="118"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
-        <v>97</v>
+      <c r="C24" s="11" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="104" t="s">
+    <row r="26" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
-      <c r="E26" s="104"/>
-      <c r="F26" s="104"/>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="104"/>
-      <c r="J26" s="104"/>
-      <c r="K26" s="104"/>
-      <c r="L26" s="104"/>
-      <c r="M26" s="104"/>
-      <c r="N26" s="104"/>
-      <c r="O26" s="104"/>
-      <c r="P26" s="104"/>
-      <c r="Q26" s="104"/>
-      <c r="R26" s="104"/>
+      <c r="D26" s="115"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="115"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="115"/>
+      <c r="J26" s="115"/>
+      <c r="K26" s="115"/>
+      <c r="L26" s="115"/>
+      <c r="M26" s="115"/>
+      <c r="N26" s="115"/>
+      <c r="O26" s="115"/>
+      <c r="P26" s="115"/>
+      <c r="Q26" s="115"/>
+      <c r="R26" s="115"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="I27" s="9"/>
     </row>
     <row r="28" spans="2:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="103" t="e">
-        <f>"3. NHS Boards provide quarterly data submissions to Public Health Scotland (PHS) on individuals diagnosed and referred for post-diagnostic support " &amp; "within their local areas and this dataset forms the basis of the LDP standard calculation. These statistics are derived from quarterly post-diagnostic support data submissions by NHS Boards as at " &amp; RIGHT(calculation!$F$6, LEN(calculation!$F$6) - 1) &amp; "."</f>
+      <c r="B28" s="114" t="s">
+        <v>169</v>
+      </c>
+      <c r="C28" s="118" t="e">
+        <f>"NHS Boards provide quarterly data submissions to Public Health Scotland (PHS) on individuals diagnosed and referred for post-diagnostic support " &amp; "within their local areas and this dataset forms the basis of the LDP standard calculation. These statistics are derived from quarterly post-diagnostic support data submissions by NHS Boards as at " &amp; RIGHT(calculation!$F$6, LEN(calculation!$F$6) - 1) &amp; "."</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C28" s="103"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="103"/>
-      <c r="F28" s="103"/>
-      <c r="G28" s="103"/>
-      <c r="H28" s="103"/>
-      <c r="I28" s="103"/>
-      <c r="J28" s="103"/>
-      <c r="K28" s="103"/>
-      <c r="L28" s="103"/>
-      <c r="M28" s="103"/>
-      <c r="N28" s="103"/>
-      <c r="O28" s="103"/>
-      <c r="P28" s="103"/>
-      <c r="Q28" s="103"/>
-      <c r="R28" s="103"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="118"/>
+      <c r="F28" s="118"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="118"/>
+      <c r="I28" s="118"/>
+      <c r="J28" s="118"/>
+      <c r="K28" s="118"/>
+      <c r="L28" s="118"/>
+      <c r="M28" s="118"/>
+      <c r="N28" s="118"/>
+      <c r="O28" s="118"/>
+      <c r="P28" s="118"/>
+      <c r="Q28" s="118"/>
+      <c r="R28" s="118"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="2:18" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="103" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" s="103"/>
-      <c r="D30" s="103"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="103"/>
-      <c r="G30" s="103"/>
-      <c r="H30" s="103"/>
-      <c r="I30" s="103"/>
-      <c r="J30" s="103"/>
-      <c r="K30" s="103"/>
-      <c r="L30" s="103"/>
-      <c r="M30" s="103"/>
-      <c r="N30" s="103"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
-    </row>
-    <row r="32" spans="2:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="103" t="s">
-        <v>115</v>
-      </c>
-      <c r="C32" s="103"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="103"/>
-      <c r="H32" s="103"/>
-      <c r="I32" s="103"/>
-      <c r="J32" s="103"/>
-      <c r="K32" s="103"/>
-      <c r="L32" s="103"/>
-      <c r="M32" s="103"/>
-      <c r="N32" s="103"/>
-      <c r="O32" s="103"/>
-      <c r="P32" s="103"/>
-      <c r="Q32" s="103"/>
-      <c r="R32" s="103"/>
-    </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
-    </row>
-    <row r="35" spans="2:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="103" t="str">
-        <f xml:space="preserve"> "6. Figures for " &amp; calculation!F8 &amp; " are provisional subject to all service users completing their support. Service users for whom it is not yet known if they have met the standard are excluded from the percentage figures."</f>
-        <v>6. Figures for  are provisional subject to all service users completing their support. Service users for whom it is not yet known if they have met the standard are excluded from the percentage figures.</v>
-      </c>
-      <c r="C35" s="103"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="103"/>
-      <c r="G35" s="103"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="103"/>
-      <c r="K35" s="103"/>
-      <c r="L35" s="103"/>
-      <c r="M35" s="103"/>
-      <c r="N35" s="103"/>
-      <c r="O35" s="103"/>
-      <c r="P35" s="103"/>
-      <c r="Q35" s="103"/>
-      <c r="R35" s="103"/>
-    </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B38" s="10"/>
-    </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B45" s="10"/>
-    </row>
-    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B47" s="10"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="10"/>
+    <row r="30" spans="2:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="114" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="118" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="118"/>
+      <c r="E30" s="118"/>
+      <c r="F30" s="118"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="118"/>
+      <c r="I30" s="118"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="118"/>
+      <c r="L30" s="118"/>
+      <c r="M30" s="118"/>
+      <c r="N30" s="118"/>
+      <c r="O30" s="118"/>
+      <c r="P30" s="118"/>
+      <c r="Q30" s="118"/>
+      <c r="R30" s="118"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="126" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="12"/>
+    </row>
+    <row r="33" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="114" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="118" t="str">
+        <f xml:space="preserve"> "Figures for " &amp; calculation!F8 &amp; " are provisional subject to all service users completing their support. Service users for whom it is not yet known if they have met the standard are excluded from the percentage figures."</f>
+        <v>Figures for  are provisional subject to all service users completing their support. Service users for whom it is not yet known if they have met the standard are excluded from the percentage figures.</v>
+      </c>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
+      <c r="F33" s="118"/>
+      <c r="G33" s="118"/>
+      <c r="H33" s="118"/>
+      <c r="I33" s="118"/>
+      <c r="J33" s="118"/>
+      <c r="K33" s="118"/>
+      <c r="L33" s="118"/>
+      <c r="M33" s="118"/>
+      <c r="N33" s="118"/>
+      <c r="O33" s="118"/>
+      <c r="P33" s="118"/>
+      <c r="Q33" s="118"/>
+      <c r="R33" s="118"/>
+    </row>
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B35" s="114" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="112" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B36" s="10"/>
+    </row>
+    <row r="37" spans="2:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="114" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="118" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="118"/>
+      <c r="E37" s="118"/>
+      <c r="F37" s="118"/>
+      <c r="G37" s="118"/>
+      <c r="H37" s="118"/>
+      <c r="I37" s="118"/>
+      <c r="J37" s="118"/>
+      <c r="K37" s="118"/>
+      <c r="L37" s="118"/>
+      <c r="M37" s="118"/>
+      <c r="N37" s="118"/>
+      <c r="O37" s="118"/>
+      <c r="P37" s="118"/>
+      <c r="Q37" s="118"/>
+      <c r="R37" s="118"/>
+    </row>
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B38" s="119"/>
+      <c r="C38" s="119"/>
+      <c r="D38" s="119"/>
+      <c r="E38" s="119"/>
+      <c r="F38" s="119"/>
+      <c r="G38" s="119"/>
+      <c r="H38" s="119"/>
+      <c r="I38" s="119"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="119"/>
+      <c r="L38" s="119"/>
+      <c r="M38" s="119"/>
+      <c r="N38" s="119"/>
+      <c r="O38" s="119"/>
+      <c r="P38" s="119"/>
+      <c r="Q38" s="119"/>
+      <c r="R38" s="119"/>
+    </row>
+    <row r="39" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="114" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" s="117" t="s">
+        <v>159</v>
+      </c>
+      <c r="D39" s="117"/>
+      <c r="E39" s="117"/>
+      <c r="F39" s="117"/>
+      <c r="G39" s="117"/>
+      <c r="H39" s="117"/>
+      <c r="I39" s="117"/>
+      <c r="J39" s="117"/>
+      <c r="K39" s="117"/>
+      <c r="L39" s="117"/>
+      <c r="M39" s="117"/>
+      <c r="N39" s="117"/>
+      <c r="O39" s="117"/>
+      <c r="P39" s="117"/>
+      <c r="Q39" s="117"/>
+      <c r="R39" s="117"/>
+    </row>
+    <row r="41" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="112"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="116"/>
+      <c r="F41" s="116"/>
+      <c r="G41" s="116"/>
+      <c r="H41" s="116"/>
+      <c r="I41" s="116"/>
+      <c r="J41" s="116"/>
+      <c r="K41" s="116"/>
+      <c r="L41" s="116"/>
+      <c r="M41" s="116"/>
+      <c r="N41" s="116"/>
+      <c r="O41" s="116"/>
+      <c r="P41" s="116"/>
+      <c r="Q41" s="116"/>
+      <c r="R41" s="116"/>
+      <c r="S41" s="116"/>
+    </row>
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B42" s="112"/>
+    </row>
+    <row r="43" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B43" s="112"/>
+    </row>
+    <row r="44" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B44" s="7"/>
+      <c r="C44" s="30"/>
+    </row>
+    <row r="45" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B35:R35"/>
-    <mergeCell ref="B32:R32"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B30:R30"/>
-    <mergeCell ref="B28:R28"/>
+  <mergeCells count="7">
+    <mergeCell ref="C39:R39"/>
+    <mergeCell ref="C37:R37"/>
+    <mergeCell ref="B38:R38"/>
+    <mergeCell ref="C23:R23"/>
+    <mergeCell ref="C28:R28"/>
+    <mergeCell ref="C30:R30"/>
+    <mergeCell ref="C33:R33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B33" r:id="rId1"/>
+    <hyperlink ref="C31" r:id="rId1"/>
     <hyperlink ref="C9" location="'Tab 1'!A1" display="Tab 1"/>
     <hyperlink ref="C10" location="'Tab 2'!A1" display="Tab 2"/>
     <hyperlink ref="C12" location="'Tab 4'!A1" display="Tab 4"/>
@@ -13983,15 +14119,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="110" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="I1" s="111" t="s">
-        <v>148</v>
-      </c>
-      <c r="J1" s="111"/>
+      <c r="A1" s="124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="I1" s="125" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="125"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
@@ -14054,7 +14190,7 @@
         <v>#N/A</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I5">
         <v>4</v>
@@ -14069,7 +14205,7 @@
         <v>#N/A</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F6" s="47"/>
       <c r="I6" s="47">
@@ -14093,7 +14229,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E8" s="47" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I8">
         <v>7</v>
@@ -14103,8 +14239,8 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E9" s="114" t="s">
-        <v>156</v>
+      <c r="E9" s="105" t="s">
+        <v>152</v>
       </c>
       <c r="I9">
         <v>8</v>
@@ -14122,7 +14258,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F11" s="115"/>
+      <c r="F11" s="106"/>
       <c r="I11">
         <v>10</v>
       </c>
@@ -14139,7 +14275,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F13" s="115"/>
+      <c r="F13" s="106"/>
       <c r="I13">
         <v>12</v>
       </c>
@@ -14426,7 +14562,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q49"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -14455,7 +14591,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -14492,7 +14628,7 @@
         <v>#N/A</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>22</v>
@@ -14510,10 +14646,10 @@
         <v>26</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="16"/>
-      <c r="J7" s="120" t="e">
+      <c r="J7" s="111" t="e">
         <f>"Percentage of people referred for dementia post-diagnostic support who received a minimum of one year’s support; " &amp; $A$7</f>
         <v>#N/A</v>
       </c>
@@ -15118,7 +15254,7 @@
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M29" s="30"/>
       <c r="N29" s="30"/>
@@ -15127,7 +15263,7 @@
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M30" s="30"/>
       <c r="N30" s="30"/>
@@ -15135,6 +15271,9 @@
       <c r="P30" s="21"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31" s="30" t="s">
+        <v>162</v>
+      </c>
       <c r="M31" s="30"/>
       <c r="N31" s="30"/>
       <c r="O31" s="30"/>
@@ -15213,9 +15352,6 @@
       <c r="P43" s="21"/>
     </row>
     <row r="44" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J44" s="29"/>
-      <c r="K44" s="30"/>
-      <c r="L44" s="30"/>
       <c r="M44" s="30"/>
       <c r="N44" s="30"/>
       <c r="O44" s="30"/>
@@ -15258,13 +15394,22 @@
       <c r="P48" s="21"/>
     </row>
     <row r="49" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J49" s="27"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
-      <c r="N49" s="21"/>
-      <c r="O49" s="21"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="30"/>
+      <c r="N49" s="30"/>
+      <c r="O49" s="30"/>
       <c r="P49" s="21"/>
+    </row>
+    <row r="50" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J50" s="27"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="21"/>
+      <c r="N50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -15279,7 +15424,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5" r:id="rId3" name="Drop Down 1">
+            <control shapeId="2" r:id="rId3" name="Drop Down 1">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -15310,7 +15455,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q79"/>
+  <dimension ref="A1:Q80"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -15339,7 +15484,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -15368,7 +15513,7 @@
         <v>#N/A</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>22</v>
@@ -15386,10 +15531,10 @@
         <v>26</v>
       </c>
       <c r="H7" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="16"/>
-      <c r="J7" s="120" t="e">
+      <c r="J7" s="111" t="e">
         <f>"Percentage of people referred for dementia post-diagnostic support who received a minimum of one year’s support; " &amp; $A$7</f>
         <v>#N/A</v>
       </c>
@@ -16655,7 +16800,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B46" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M46" s="30"/>
       <c r="N46" s="30"/>
@@ -16664,7 +16809,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M47" s="30"/>
       <c r="N47" s="30"/>
@@ -16672,22 +16817,16 @@
       <c r="P47" s="21"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B48" s="30"/>
+      <c r="B48" s="30" t="s">
+        <v>164</v>
+      </c>
       <c r="M48" s="30"/>
       <c r="N48" s="30"/>
       <c r="O48" s="30"/>
       <c r="P48" s="21"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="30"/>
+      <c r="B49" s="112"/>
       <c r="M49" s="30"/>
       <c r="N49" s="30"/>
       <c r="O49" s="30"/>
@@ -16958,15 +17097,30 @@
       <c r="G67" s="30"/>
       <c r="H67" s="30"/>
       <c r="I67" s="30"/>
-      <c r="M67" s="21"/>
-      <c r="N67" s="21"/>
-      <c r="O67" s="21"/>
+      <c r="M67" s="30"/>
+      <c r="N67" s="30"/>
+      <c r="O67" s="30"/>
       <c r="P67" s="21"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J79" s="29"/>
-      <c r="K79" s="30"/>
-      <c r="L79" s="30"/>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="14"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="30"/>
+      <c r="M68" s="21"/>
+      <c r="N68" s="21"/>
+      <c r="O68" s="21"/>
+      <c r="P68" s="21"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J80" s="29"/>
+      <c r="K80" s="30"/>
+      <c r="L80" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -16981,7 +17135,7 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="5" r:id="rId3" name="Drop Down 1">
+            <control shapeId="2" r:id="rId3" name="Drop Down 1">
               <controlPr defaultSize="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -17034,13 +17188,13 @@
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -17068,7 +17222,7 @@
         <v>NHS Ayrshire &amp; Arran</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C5" s="86" t="e">
         <f>calculation!$C2</f>
@@ -17084,7 +17238,7 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="100" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K5" s="99"/>
       <c r="L5" s="16"/>
@@ -17178,7 +17332,7 @@
       </c>
       <c r="F9" s="88"/>
       <c r="G9" s="48" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H9" s="48" t="str">
         <f>"Percentage of people referred for dementia post-diagnostic support who received a minimum of one year’s support; " &amp; $A$5 &amp; " and Scotland"</f>
@@ -17208,7 +17362,7 @@
       </c>
       <c r="F10" s="88"/>
       <c r="G10" s="48" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H10" s="101">
         <f>calculation!$B2</f>
@@ -18391,7 +18545,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B59" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J59" s="30"/>
       <c r="K59" s="30"/>
@@ -18400,7 +18554,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B60" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J60" s="30"/>
       <c r="K60" s="30"/>
@@ -18408,7 +18562,9 @@
       <c r="M60" s="21"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B61" s="30"/>
+      <c r="B61" s="30" t="s">
+        <v>161</v>
+      </c>
       <c r="J61" s="30"/>
       <c r="K61" s="30"/>
       <c r="L61" s="30"/>
@@ -18691,7 +18847,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AA42"/>
+  <dimension ref="A1:AA43"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -18721,7 +18877,7 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -18809,7 +18965,7 @@
         <v>#N/A</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>22</v>
@@ -18830,10 +18986,10 @@
         <v>26</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J7" s="16"/>
-      <c r="K7" s="120" t="e">
+      <c r="K7" s="111" t="e">
         <f>"Proportion of total referrals for dementia post-diagnostic support; "&amp;A7</f>
         <v>#N/A</v>
       </c>
@@ -18850,7 +19006,7 @@
         <v>29</v>
       </c>
       <c r="T7" s="14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="U7" s="48"/>
       <c r="V7" s="47"/>
@@ -18893,7 +19049,7 @@
         <v>-</v>
       </c>
       <c r="J8" s="30"/>
-      <c r="K8" s="120" t="e">
+      <c r="K8" s="111" t="e">
         <f>"Percentage of people referred for dementia post-diagnostic support who received a minimum of one year’s support; "&amp;A7</f>
         <v>#N/A</v>
       </c>
@@ -19345,7 +19501,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" s="45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="19" t="e">
         <f t="shared" ca="1" si="5"/>
@@ -19433,7 +19589,7 @@
         <v>#N/A</v>
       </c>
       <c r="I17" s="26" t="e">
-        <f t="shared" ref="I9:I17" ca="1" si="11">(E17+F17)/(C17-G17)</f>
+        <f t="shared" ref="I17" ca="1" si="11">(E17+F17)/(C17-G17)</f>
         <v>#N/A</v>
       </c>
       <c r="J17" s="30"/>
@@ -19643,7 +19799,7 @@
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -19674,7 +19830,7 @@
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -19705,7 +19861,7 @@
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
@@ -19735,7 +19891,9 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
-      <c r="B27" s="30"/>
+      <c r="B27" s="113" t="s">
+        <v>163</v>
+      </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
@@ -19753,7 +19911,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
-      <c r="B28" s="30"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
@@ -19925,9 +20083,6 @@
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
       <c r="K37" s="29"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="30"/>
-      <c r="N37" s="30"/>
       <c r="O37" s="30"/>
       <c r="P37" s="30"/>
       <c r="Q37" s="30"/>
@@ -20029,15 +20184,36 @@
       <c r="H42" s="30"/>
       <c r="I42" s="30"/>
       <c r="J42" s="30"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
-      <c r="N42" s="21"/>
-      <c r="O42" s="21"/>
-      <c r="P42" s="21"/>
-      <c r="Q42" s="21"/>
-      <c r="R42" s="21"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="30"/>
+      <c r="M42" s="30"/>
+      <c r="N42" s="30"/>
+      <c r="O42" s="30"/>
+      <c r="P42" s="30"/>
+      <c r="Q42" s="30"/>
+      <c r="R42" s="30"/>
       <c r="S42" s="21"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="14"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -20083,7 +20259,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U40"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -20113,7 +20289,7 @@
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
@@ -20166,7 +20342,7 @@
         <v>#N/A</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>22</v>
@@ -20187,10 +20363,10 @@
         <v>26</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J7" s="51"/>
-      <c r="K7" s="120" t="e">
+      <c r="K7" s="111" t="e">
         <f>"Proportion of total referrals for dementia post-diagnostic support; "&amp;A7</f>
         <v>#N/A</v>
       </c>
@@ -20238,7 +20414,7 @@
         <v>-</v>
       </c>
       <c r="J8" s="49"/>
-      <c r="K8" s="120" t="e">
+      <c r="K8" s="111" t="e">
         <f>"Percentage of people referred for dementia post-diagnostic support who received a minimum of one year’s support; "&amp;A7</f>
         <v>#N/A</v>
       </c>
@@ -20435,7 +20611,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="53" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="19" t="e">
         <f t="shared" ca="1" si="6"/>
@@ -20508,7 +20684,7 @@
         <v>#N/A</v>
       </c>
       <c r="I14" s="26" t="e">
-        <f t="shared" ref="I9:I14" ca="1" si="8">(E14+F14)/(C14-G14)</f>
+        <f t="shared" ref="I14" ca="1" si="8">(E14+F14)/(C14-G14)</f>
         <v>#N/A</v>
       </c>
       <c r="J14" s="49"/>
@@ -20664,7 +20840,7 @@
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -20687,7 +20863,7 @@
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -20710,7 +20886,7 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="30"/>
@@ -20733,7 +20909,7 @@
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="55" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="30"/>
       <c r="D24" s="30"/>
@@ -20755,7 +20931,9 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
-      <c r="B25" s="30"/>
+      <c r="B25" s="113" t="s">
+        <v>163</v>
+      </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -20763,12 +20941,15 @@
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
       <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="29"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49"/>
+      <c r="O25" s="49"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="49"/>
+      <c r="R25" s="49"/>
       <c r="S25" s="21"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -20945,9 +21126,6 @@
       <c r="I35" s="30"/>
       <c r="J35" s="30"/>
       <c r="K35" s="29"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
       <c r="O35" s="30"/>
       <c r="P35" s="30"/>
       <c r="Q35" s="30"/>
@@ -21049,15 +21227,36 @@
       <c r="H40" s="30"/>
       <c r="I40" s="30"/>
       <c r="J40" s="30"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
-      <c r="N40" s="21"/>
-      <c r="O40" s="21"/>
-      <c r="P40" s="21"/>
-      <c r="Q40" s="21"/>
-      <c r="R40" s="21"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="30"/>
+      <c r="M40" s="30"/>
+      <c r="N40" s="30"/>
+      <c r="O40" s="30"/>
+      <c r="P40" s="30"/>
+      <c r="Q40" s="30"/>
+      <c r="R40" s="30"/>
       <c r="S40" s="21"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
+      <c r="B41" s="30"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="30"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="30"/>
+      <c r="J41" s="30"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -21139,7 +21338,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="68" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C3" s="59"/>
       <c r="D3" s="30"/>
@@ -21188,7 +21387,7 @@
         <v>#N/A</v>
       </c>
       <c r="B7" s="57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>21</v>
@@ -21197,9 +21396,9 @@
         <v>22</v>
       </c>
       <c r="E7" s="71" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="120" t="e">
+        <v>105</v>
+      </c>
+      <c r="G7" s="111" t="e">
         <f>$E$7&amp;"; "&amp;$A$7</f>
         <v>#N/A</v>
       </c>
@@ -21595,7 +21794,7 @@
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="70" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -21680,7 +21879,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="58" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="J29" s="29"/>
       <c r="K29" s="30"/>
@@ -21691,7 +21890,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" s="69" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J30" s="29"/>
       <c r="K30" s="30"/>
@@ -21702,7 +21901,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="58" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J31" s="29"/>
       <c r="K31" s="30"/>
@@ -22082,13 +22281,13 @@
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="72" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -22116,7 +22315,7 @@
         <v>NHS Ayrshire &amp; Arran</v>
       </c>
       <c r="B5" s="85" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C5" s="86" t="e">
         <f>calculation!$C2</f>
@@ -22132,7 +22331,7 @@
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="100" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="K5" s="99"/>
       <c r="L5" s="16"/>
@@ -22226,7 +22425,7 @@
       </c>
       <c r="F9" s="88"/>
       <c r="G9" s="48" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H9" s="48" t="str">
         <f>"Percentage of people estimated to be newly diagnosed with dementia who were referred for post-diagnostic support; " &amp; $A$5 &amp; " and Scotland"</f>
@@ -22256,7 +22455,7 @@
       </c>
       <c r="F10" s="88"/>
       <c r="G10" s="48" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H10" s="101">
         <f>calculation!$B2</f>
@@ -22587,13 +22786,13 @@
       <c r="M21" s="21"/>
     </row>
     <row r="22" spans="1:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="106" t="e">
+      <c r="B22" s="120" t="e">
         <f xml:space="preserve"> "Source: Public Health Scotland quarterly dementia post-diagnostic support dataset: Data submissions from NHS Boards as at " &amp; RIGHT(calculation!$F$6, LEN(calculation!$F$6) - 1) &amp; ".  Estimated and Projected Diagnosis Rates for Dementia in Scotland paper: 2014-2020."</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="120"/>
+      <c r="E22" s="120"/>
       <c r="G22" s="29"/>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
@@ -22603,8 +22802,8 @@
       <c r="M22" s="21"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="117" t="s">
-        <v>159</v>
+      <c r="B23" s="108" t="s">
+        <v>155</v>
       </c>
       <c r="C23" s="28"/>
       <c r="G23" s="29"/>
@@ -22616,7 +22815,7 @@
       <c r="M23" s="21"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="116" t="s">
+      <c r="B24" s="107" t="s">
         <v>70</v>
       </c>
       <c r="C24" s="28"/>
@@ -22652,8 +22851,8 @@
       <c r="M26" s="21"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="118" t="s">
-        <v>121</v>
+      <c r="B27" s="109" t="s">
+        <v>117</v>
       </c>
       <c r="J27" s="30"/>
       <c r="K27" s="30"/>
@@ -22661,8 +22860,8 @@
       <c r="M27" s="21"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="119" t="s">
-        <v>131</v>
+      <c r="B28" s="110" t="s">
+        <v>127</v>
       </c>
       <c r="J28" s="30"/>
       <c r="K28" s="30"/>
@@ -22671,8 +22870,8 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="96"/>
-      <c r="B29" s="118" t="s">
-        <v>158</v>
+      <c r="B29" s="109" t="s">
+        <v>154</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -39353,7 +39552,7 @@
     </row>
     <row r="4" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="B4" s="76" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:16383" x14ac:dyDescent="0.25">
@@ -39399,7 +39598,7 @@
     </row>
     <row r="14" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="B14" s="76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:16383" x14ac:dyDescent="0.25">
@@ -39465,29 +39664,29 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="76" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" s="108" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="108"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="108"/>
-      <c r="G29" s="108"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="108"/>
+        <v>113</v>
+      </c>
+      <c r="C29" s="122" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" s="122"/>
+      <c r="E29" s="122"/>
+      <c r="F29" s="122"/>
+      <c r="G29" s="122"/>
+      <c r="H29" s="122"/>
+      <c r="I29" s="122"/>
       <c r="J29" s="74" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K29" s="74"/>
       <c r="L29" s="74"/>
@@ -39496,15 +39695,15 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="74"/>
-      <c r="C30" s="109" t="s">
-        <v>113</v>
-      </c>
-      <c r="D30" s="109"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="109"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="109"/>
-      <c r="I30" s="109"/>
+      <c r="C30" s="123" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="123"/>
+      <c r="E30" s="123"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="123"/>
+      <c r="H30" s="123"/>
+      <c r="I30" s="123"/>
       <c r="J30" s="74"/>
       <c r="K30" s="74"/>
       <c r="L30" s="74"/>
@@ -39528,98 +39727,98 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B32" s="30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="121" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="34" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="107" t="s">
+      <c r="C34" s="121"/>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="F34" s="121"/>
+      <c r="G34" s="121"/>
+      <c r="H34" s="121"/>
+      <c r="I34" s="121"/>
+      <c r="J34" s="121"/>
+      <c r="K34" s="121"/>
+      <c r="L34" s="121"/>
+      <c r="M34" s="121"/>
+      <c r="N34" s="121"/>
+      <c r="O34" s="121"/>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B35" s="121" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="121"/>
+      <c r="D35" s="121"/>
+      <c r="E35" s="121"/>
+      <c r="F35" s="121"/>
+      <c r="G35" s="121"/>
+      <c r="H35" s="121"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="121"/>
+      <c r="K35" s="121"/>
+      <c r="L35" s="121"/>
+      <c r="M35" s="121"/>
+      <c r="N35" s="121"/>
+      <c r="O35" s="121"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B36" s="121" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="F36" s="121"/>
+      <c r="G36" s="121"/>
+      <c r="H36" s="121"/>
+      <c r="I36" s="121"/>
+      <c r="J36" s="121"/>
+      <c r="K36" s="121"/>
+      <c r="L36" s="121"/>
+      <c r="M36" s="121"/>
+      <c r="N36" s="121"/>
+      <c r="O36" s="121"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="121" t="s">
         <v>123</v>
       </c>
-      <c r="C34" s="107"/>
-      <c r="D34" s="107"/>
-      <c r="E34" s="107"/>
-      <c r="F34" s="107"/>
-      <c r="G34" s="107"/>
-      <c r="H34" s="107"/>
-      <c r="I34" s="107"/>
-      <c r="J34" s="107"/>
-      <c r="K34" s="107"/>
-      <c r="L34" s="107"/>
-      <c r="M34" s="107"/>
-      <c r="N34" s="107"/>
-      <c r="O34" s="107"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="107" t="s">
-        <v>125</v>
-      </c>
-      <c r="C35" s="107"/>
-      <c r="D35" s="107"/>
-      <c r="E35" s="107"/>
-      <c r="F35" s="107"/>
-      <c r="G35" s="107"/>
-      <c r="H35" s="107"/>
-      <c r="I35" s="107"/>
-      <c r="J35" s="107"/>
-      <c r="K35" s="107"/>
-      <c r="L35" s="107"/>
-      <c r="M35" s="107"/>
-      <c r="N35" s="107"/>
-      <c r="O35" s="107"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="107" t="s">
-        <v>126</v>
-      </c>
-      <c r="C36" s="107"/>
-      <c r="D36" s="107"/>
-      <c r="E36" s="107"/>
-      <c r="F36" s="107"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="107"/>
-      <c r="I36" s="107"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="107"/>
-      <c r="N36" s="107"/>
-      <c r="O36" s="107"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="107" t="s">
-        <v>127</v>
-      </c>
-      <c r="C37" s="107"/>
-      <c r="D37" s="107"/>
-      <c r="E37" s="107"/>
-      <c r="F37" s="107"/>
-      <c r="G37" s="107"/>
-      <c r="H37" s="107"/>
-      <c r="I37" s="107"/>
-      <c r="J37" s="107"/>
-      <c r="K37" s="107"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="107"/>
-      <c r="N37" s="107"/>
-      <c r="O37" s="107"/>
+      <c r="C37" s="121"/>
+      <c r="D37" s="121"/>
+      <c r="E37" s="121"/>
+      <c r="F37" s="121"/>
+      <c r="G37" s="121"/>
+      <c r="H37" s="121"/>
+      <c r="I37" s="121"/>
+      <c r="J37" s="121"/>
+      <c r="K37" s="121"/>
+      <c r="L37" s="121"/>
+      <c r="M37" s="121"/>
+      <c r="N37" s="121"/>
+      <c r="O37" s="121"/>
     </row>
     <row r="38" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="107" t="s">
-        <v>124</v>
-      </c>
-      <c r="C38" s="107"/>
-      <c r="D38" s="107"/>
-      <c r="E38" s="107"/>
-      <c r="F38" s="107"/>
-      <c r="G38" s="107"/>
-      <c r="H38" s="107"/>
-      <c r="I38" s="107"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="107"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="107"/>
-      <c r="O38" s="107"/>
+      <c r="B38" s="121" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="121"/>
+      <c r="D38" s="121"/>
+      <c r="E38" s="121"/>
+      <c r="F38" s="121"/>
+      <c r="G38" s="121"/>
+      <c r="H38" s="121"/>
+      <c r="I38" s="121"/>
+      <c r="J38" s="121"/>
+      <c r="K38" s="121"/>
+      <c r="L38" s="121"/>
+      <c r="M38" s="121"/>
+      <c r="N38" s="121"/>
+      <c r="O38" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Updates to excel notes
</commit_message>
<xml_diff>
--- a/reference-files/excel-template.xlsx
+++ b/reference-files/excel-template.xlsx
@@ -657,9 +657,6 @@
     <t>As a result of the COVID-19 pandemic, some areas have reported difficulties in updating their data systems which are required to provide the dementia PDS dataset, however it is not anticipated that this has a large impact on the data presented in this report.</t>
   </si>
   <si>
-    <t>Aberdeen City Health &amp; Social Care Partnership ceased its contract with Alzheimer Scotland during 2019 and introduced an in house dementia PDS service. This transition resulted in some PDS cases being terminated by Alzheimer Scotland earlier than 12 months and therefore not meeting the LDP standard. As part of the transition, individuals were contacted to ask if they still wanted to receive PDS which was then provided by the in house service, if required. This should be taken into account when interpreting figures for 2018/19.</t>
-  </si>
-  <si>
     <t>2018/19 figures for NHS Grampian and Aberdeen City are affected by a change in service provision of PDS within Aberdeen City during 2019. See Notes tab for further information.</t>
   </si>
   <si>
@@ -676,9 +673,6 @@
   </si>
   <si>
     <t>These tables are supplementary to the full publication report which can be found at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Scottish Government published their third national dementia strategy in 2017. This included the commitment to extend and embed dementia post-diagnostic support. In order to effectively monitor the delivery of post-diagnosis support a national local delivery plan (LDP) standard was introduced for all those newly diagnosed with dementia to receive a minimum of one year’s post-diagnostic support. </t>
   </si>
   <si>
     <t>2/</t>
@@ -703,6 +697,12 @@
   </si>
   <si>
     <t>8/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Scottish Government published their third national dementia strategy in 2017. This included the commitment to extend and embed dementia post-diagnostic support. In order to effectively monitor the delivery of post-diagnosis support a national local delivery plan (LDP) standard was introduced for all people newly diagnosed with dementia to receive a minimum of one year’s post-diagnostic support. </t>
+  </si>
+  <si>
+    <t>Aberdeen City Health &amp; Social Care Partnership ceased its contract with Alzheimer Scotland during 2019 and introduced an in-house dementia PDS service. This transition resulted in some PDS cases being terminated by Alzheimer Scotland earlier than 12 months and therefore not meeting the LDP standard. As part of the transition, individuals were contacted to ask if they still wanted to receive PDS which was then provided by the in-house service, if required. This should be taken into account when interpreting figures for 2018/19.</t>
   </si>
 </sst>
 </file>
@@ -1350,6 +1350,9 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1376,9 +1379,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1430,6 +1430,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1548,6 +1549,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -12415,10 +12417,10 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>165</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -12429,26 +12431,26 @@
     </row>
     <row r="23" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="114" t="s">
-        <v>168</v>
-      </c>
-      <c r="C23" s="118" t="s">
-        <v>167</v>
-      </c>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="118"/>
-      <c r="J23" s="118"/>
-      <c r="K23" s="118"/>
-      <c r="L23" s="118"/>
-      <c r="M23" s="118"/>
-      <c r="N23" s="118"/>
-      <c r="O23" s="118"/>
-      <c r="P23" s="118"/>
-      <c r="Q23" s="118"/>
-      <c r="R23" s="118"/>
+        <v>166</v>
+      </c>
+      <c r="C23" s="119" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="119"/>
+      <c r="O23" s="119"/>
+      <c r="P23" s="119"/>
+      <c r="Q23" s="119"/>
+      <c r="R23" s="119"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C24" s="11" t="s">
@@ -12486,56 +12488,56 @@
     </row>
     <row r="28" spans="2:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="114" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28" s="118" t="e">
+        <v>167</v>
+      </c>
+      <c r="C28" s="119" t="e">
         <f>"NHS Boards provide quarterly data submissions to Public Health Scotland (PHS) on individuals diagnosed and referred for post-diagnostic support " &amp; "within their local areas and this dataset forms the basis of the LDP standard calculation. These statistics are derived from quarterly post-diagnostic support data submissions by NHS Boards as at " &amp; RIGHT(calculation!$F$6, LEN(calculation!$F$6) - 1) &amp; "."</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="118"/>
-      <c r="M28" s="118"/>
-      <c r="N28" s="118"/>
-      <c r="O28" s="118"/>
-      <c r="P28" s="118"/>
-      <c r="Q28" s="118"/>
-      <c r="R28" s="118"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="119"/>
+      <c r="I28" s="119"/>
+      <c r="J28" s="119"/>
+      <c r="K28" s="119"/>
+      <c r="L28" s="119"/>
+      <c r="M28" s="119"/>
+      <c r="N28" s="119"/>
+      <c r="O28" s="119"/>
+      <c r="P28" s="119"/>
+      <c r="Q28" s="119"/>
+      <c r="R28" s="119"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
     <row r="30" spans="2:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="114" t="s">
-        <v>171</v>
-      </c>
-      <c r="C30" s="118" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="118"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="118"/>
-      <c r="M30" s="118"/>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
-      <c r="P30" s="118"/>
-      <c r="Q30" s="118"/>
-      <c r="R30" s="118"/>
+        <v>169</v>
+      </c>
+      <c r="C30" s="119" t="s">
+        <v>168</v>
+      </c>
+      <c r="D30" s="119"/>
+      <c r="E30" s="119"/>
+      <c r="F30" s="119"/>
+      <c r="G30" s="119"/>
+      <c r="H30" s="119"/>
+      <c r="I30" s="119"/>
+      <c r="J30" s="119"/>
+      <c r="K30" s="119"/>
+      <c r="L30" s="119"/>
+      <c r="M30" s="119"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="119"/>
+      <c r="P30" s="119"/>
+      <c r="Q30" s="119"/>
+      <c r="R30" s="119"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="C31" s="126" t="s">
+      <c r="C31" s="117" t="s">
         <v>127</v>
       </c>
     </row>
@@ -12544,31 +12546,31 @@
     </row>
     <row r="33" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="114" t="s">
-        <v>172</v>
-      </c>
-      <c r="C33" s="118" t="str">
+        <v>170</v>
+      </c>
+      <c r="C33" s="119" t="str">
         <f xml:space="preserve"> "Figures for " &amp; calculation!F8 &amp; " are provisional subject to all service users completing their support. Service users for whom it is not yet known if they have met the standard are excluded from the percentage figures."</f>
         <v>Figures for  are provisional subject to all service users completing their support. Service users for whom it is not yet known if they have met the standard are excluded from the percentage figures.</v>
       </c>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="118"/>
-      <c r="K33" s="118"/>
-      <c r="L33" s="118"/>
-      <c r="M33" s="118"/>
-      <c r="N33" s="118"/>
-      <c r="O33" s="118"/>
-      <c r="P33" s="118"/>
-      <c r="Q33" s="118"/>
-      <c r="R33" s="118"/>
+      <c r="D33" s="119"/>
+      <c r="E33" s="119"/>
+      <c r="F33" s="119"/>
+      <c r="G33" s="119"/>
+      <c r="H33" s="119"/>
+      <c r="I33" s="119"/>
+      <c r="J33" s="119"/>
+      <c r="K33" s="119"/>
+      <c r="L33" s="119"/>
+      <c r="M33" s="119"/>
+      <c r="N33" s="119"/>
+      <c r="O33" s="119"/>
+      <c r="P33" s="119"/>
+      <c r="Q33" s="119"/>
+      <c r="R33" s="119"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B35" s="114" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C35" s="112" t="s">
         <v>158</v>
@@ -12579,68 +12581,68 @@
     </row>
     <row r="37" spans="2:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="114" t="s">
-        <v>174</v>
-      </c>
-      <c r="C37" s="118" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="118"/>
-      <c r="L37" s="118"/>
-      <c r="M37" s="118"/>
-      <c r="N37" s="118"/>
-      <c r="O37" s="118"/>
-      <c r="P37" s="118"/>
-      <c r="Q37" s="118"/>
-      <c r="R37" s="118"/>
+        <v>172</v>
+      </c>
+      <c r="C37" s="119" t="s">
+        <v>175</v>
+      </c>
+      <c r="D37" s="119"/>
+      <c r="E37" s="119"/>
+      <c r="F37" s="119"/>
+      <c r="G37" s="119"/>
+      <c r="H37" s="119"/>
+      <c r="I37" s="119"/>
+      <c r="J37" s="119"/>
+      <c r="K37" s="119"/>
+      <c r="L37" s="119"/>
+      <c r="M37" s="119"/>
+      <c r="N37" s="119"/>
+      <c r="O37" s="119"/>
+      <c r="P37" s="119"/>
+      <c r="Q37" s="119"/>
+      <c r="R37" s="119"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B38" s="119"/>
-      <c r="C38" s="119"/>
-      <c r="D38" s="119"/>
-      <c r="E38" s="119"/>
-      <c r="F38" s="119"/>
-      <c r="G38" s="119"/>
-      <c r="H38" s="119"/>
-      <c r="I38" s="119"/>
-      <c r="J38" s="119"/>
-      <c r="K38" s="119"/>
-      <c r="L38" s="119"/>
-      <c r="M38" s="119"/>
-      <c r="N38" s="119"/>
-      <c r="O38" s="119"/>
-      <c r="P38" s="119"/>
-      <c r="Q38" s="119"/>
-      <c r="R38" s="119"/>
+      <c r="B38" s="120"/>
+      <c r="C38" s="120"/>
+      <c r="D38" s="120"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="120"/>
+      <c r="G38" s="120"/>
+      <c r="H38" s="120"/>
+      <c r="I38" s="120"/>
+      <c r="J38" s="120"/>
+      <c r="K38" s="120"/>
+      <c r="L38" s="120"/>
+      <c r="M38" s="120"/>
+      <c r="N38" s="120"/>
+      <c r="O38" s="120"/>
+      <c r="P38" s="120"/>
+      <c r="Q38" s="120"/>
+      <c r="R38" s="120"/>
     </row>
     <row r="39" spans="2:19" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="114" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="117" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="118" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="117"/>
-      <c r="E39" s="117"/>
-      <c r="F39" s="117"/>
-      <c r="G39" s="117"/>
-      <c r="H39" s="117"/>
-      <c r="I39" s="117"/>
-      <c r="J39" s="117"/>
-      <c r="K39" s="117"/>
-      <c r="L39" s="117"/>
-      <c r="M39" s="117"/>
-      <c r="N39" s="117"/>
-      <c r="O39" s="117"/>
-      <c r="P39" s="117"/>
-      <c r="Q39" s="117"/>
-      <c r="R39" s="117"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="118"/>
+      <c r="J39" s="118"/>
+      <c r="K39" s="118"/>
+      <c r="L39" s="118"/>
+      <c r="M39" s="118"/>
+      <c r="N39" s="118"/>
+      <c r="O39" s="118"/>
+      <c r="P39" s="118"/>
+      <c r="Q39" s="118"/>
+      <c r="R39" s="118"/>
     </row>
     <row r="41" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="112"/>
@@ -14119,15 +14121,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="125" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="I1" s="125" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="I1" s="126" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="125"/>
+      <c r="J1" s="126"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
@@ -15272,7 +15274,7 @@
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M31" s="30"/>
       <c r="N31" s="30"/>
@@ -16818,7 +16820,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B48" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M48" s="30"/>
       <c r="N48" s="30"/>
@@ -18563,7 +18565,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B61" s="30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J61" s="30"/>
       <c r="K61" s="30"/>
@@ -19892,7 +19894,7 @@
     <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -20932,7 +20934,7 @@
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="113" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -22786,13 +22788,13 @@
       <c r="M21" s="21"/>
     </row>
     <row r="22" spans="1:16" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="120" t="e">
+      <c r="B22" s="121" t="e">
         <f xml:space="preserve"> "Source: Public Health Scotland quarterly dementia post-diagnostic support dataset: Data submissions from NHS Boards as at " &amp; RIGHT(calculation!$F$6, LEN(calculation!$F$6) - 1) &amp; ".  Estimated and Projected Diagnosis Rates for Dementia in Scotland paper: 2014-2020."</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C22" s="120"/>
-      <c r="D22" s="120"/>
-      <c r="E22" s="120"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="121"/>
       <c r="G22" s="29"/>
       <c r="H22" s="30"/>
       <c r="I22" s="30"/>
@@ -39676,15 +39678,15 @@
       <c r="B29" s="73" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="122" t="s">
+      <c r="C29" s="123" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="122"/>
-      <c r="E29" s="122"/>
-      <c r="F29" s="122"/>
-      <c r="G29" s="122"/>
-      <c r="H29" s="122"/>
-      <c r="I29" s="122"/>
+      <c r="D29" s="123"/>
+      <c r="E29" s="123"/>
+      <c r="F29" s="123"/>
+      <c r="G29" s="123"/>
+      <c r="H29" s="123"/>
+      <c r="I29" s="123"/>
       <c r="J29" s="74" t="s">
         <v>116</v>
       </c>
@@ -39695,15 +39697,15 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="74"/>
-      <c r="C30" s="123" t="s">
+      <c r="C30" s="124" t="s">
         <v>112</v>
       </c>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="123"/>
-      <c r="I30" s="123"/>
+      <c r="D30" s="124"/>
+      <c r="E30" s="124"/>
+      <c r="F30" s="124"/>
+      <c r="G30" s="124"/>
+      <c r="H30" s="124"/>
+      <c r="I30" s="124"/>
       <c r="J30" s="74"/>
       <c r="K30" s="74"/>
       <c r="L30" s="74"/>
@@ -39731,94 +39733,94 @@
       </c>
     </row>
     <row r="34" spans="2:15" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="121" t="s">
+      <c r="B34" s="122" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="121"/>
-      <c r="D34" s="121"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="121"/>
-      <c r="G34" s="121"/>
-      <c r="H34" s="121"/>
-      <c r="I34" s="121"/>
-      <c r="J34" s="121"/>
-      <c r="K34" s="121"/>
-      <c r="L34" s="121"/>
-      <c r="M34" s="121"/>
-      <c r="N34" s="121"/>
-      <c r="O34" s="121"/>
+      <c r="C34" s="122"/>
+      <c r="D34" s="122"/>
+      <c r="E34" s="122"/>
+      <c r="F34" s="122"/>
+      <c r="G34" s="122"/>
+      <c r="H34" s="122"/>
+      <c r="I34" s="122"/>
+      <c r="J34" s="122"/>
+      <c r="K34" s="122"/>
+      <c r="L34" s="122"/>
+      <c r="M34" s="122"/>
+      <c r="N34" s="122"/>
+      <c r="O34" s="122"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="122" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="121"/>
-      <c r="D35" s="121"/>
-      <c r="E35" s="121"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="121"/>
-      <c r="I35" s="121"/>
-      <c r="J35" s="121"/>
-      <c r="K35" s="121"/>
-      <c r="L35" s="121"/>
-      <c r="M35" s="121"/>
-      <c r="N35" s="121"/>
-      <c r="O35" s="121"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="122"/>
+      <c r="F35" s="122"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="122"/>
+      <c r="I35" s="122"/>
+      <c r="J35" s="122"/>
+      <c r="K35" s="122"/>
+      <c r="L35" s="122"/>
+      <c r="M35" s="122"/>
+      <c r="N35" s="122"/>
+      <c r="O35" s="122"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="121" t="s">
+      <c r="B36" s="122" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="121"/>
-      <c r="F36" s="121"/>
-      <c r="G36" s="121"/>
-      <c r="H36" s="121"/>
-      <c r="I36" s="121"/>
-      <c r="J36" s="121"/>
-      <c r="K36" s="121"/>
-      <c r="L36" s="121"/>
-      <c r="M36" s="121"/>
-      <c r="N36" s="121"/>
-      <c r="O36" s="121"/>
+      <c r="C36" s="122"/>
+      <c r="D36" s="122"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="122"/>
+      <c r="G36" s="122"/>
+      <c r="H36" s="122"/>
+      <c r="I36" s="122"/>
+      <c r="J36" s="122"/>
+      <c r="K36" s="122"/>
+      <c r="L36" s="122"/>
+      <c r="M36" s="122"/>
+      <c r="N36" s="122"/>
+      <c r="O36" s="122"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="121" t="s">
+      <c r="B37" s="122" t="s">
         <v>123</v>
       </c>
-      <c r="C37" s="121"/>
-      <c r="D37" s="121"/>
-      <c r="E37" s="121"/>
-      <c r="F37" s="121"/>
-      <c r="G37" s="121"/>
-      <c r="H37" s="121"/>
-      <c r="I37" s="121"/>
-      <c r="J37" s="121"/>
-      <c r="K37" s="121"/>
-      <c r="L37" s="121"/>
-      <c r="M37" s="121"/>
-      <c r="N37" s="121"/>
-      <c r="O37" s="121"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="122"/>
+      <c r="E37" s="122"/>
+      <c r="F37" s="122"/>
+      <c r="G37" s="122"/>
+      <c r="H37" s="122"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="122"/>
+      <c r="K37" s="122"/>
+      <c r="L37" s="122"/>
+      <c r="M37" s="122"/>
+      <c r="N37" s="122"/>
+      <c r="O37" s="122"/>
     </row>
     <row r="38" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="121" t="s">
+      <c r="B38" s="122" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="121"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="121"/>
-      <c r="K38" s="121"/>
-      <c r="L38" s="121"/>
-      <c r="M38" s="121"/>
-      <c r="N38" s="121"/>
-      <c r="O38" s="121"/>
+      <c r="C38" s="122"/>
+      <c r="D38" s="122"/>
+      <c r="E38" s="122"/>
+      <c r="F38" s="122"/>
+      <c r="G38" s="122"/>
+      <c r="H38" s="122"/>
+      <c r="I38" s="122"/>
+      <c r="J38" s="122"/>
+      <c r="K38" s="122"/>
+      <c r="L38" s="122"/>
+      <c r="M38" s="122"/>
+      <c r="N38" s="122"/>
+      <c r="O38" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Add embargo text to excel tables
</commit_message>
<xml_diff>
--- a/reference-files/excel-template.xlsx
+++ b/reference-files/excel-template.xlsx
@@ -714,7 +714,7 @@
     <numFmt numFmtId="165" formatCode="?0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -913,6 +913,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -944,6 +945,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0D0D0D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1106,7 +1114,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -1380,6 +1388,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1430,7 +1439,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1549,7 +1557,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2431,6 +2438,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2732,6 +2740,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4827,6 +4836,7 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5126,6 +5136,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10158,7 +10169,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>511810</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -12238,7 +12249,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:S47"/>
+  <dimension ref="B1:S47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -12252,6 +12263,12 @@
     <col min="19" max="19" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:18" ht="18" x14ac:dyDescent="0.25">
+      <c r="B1" s="127" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+    </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>24</v>
@@ -14578,10 +14595,14 @@
     <col min="11" max="12" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -15471,10 +15492,14 @@
     <col min="11" max="12" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -17182,10 +17207,14 @@
     <col min="8" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="96" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -18863,10 +18892,14 @@
     <col min="12" max="14" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -20275,10 +20308,14 @@
     <col min="12" max="14" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -21320,10 +21357,14 @@
     <col min="11" max="12" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -22275,10 +22316,14 @@
     <col min="8" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="96" t="str">
+    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="127" t="str">
         <f>Notes!B2</f>
         <v xml:space="preserve"> </v>
+      </c>
+      <c r="B1" s="127" t="str">
+        <f>Notes!B1</f>
+        <v/>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>